<commit_message>
metrics in both disall and dis1 for sched and no sched
</commit_message>
<xml_diff>
--- a/VRNN_theano_version/output/vrnn-gen-dataport.xlsx
+++ b/VRNN_theano_version/output/vrnn-gen-dataport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="187">
   <si>
     <t>epochs</t>
   </si>
@@ -336,6 +336,36 @@
     <t>18-05-13_01-09</t>
   </si>
   <si>
+    <t>0:0.001,</t>
+  </si>
+  <si>
+    <t>18-05-15_11-11</t>
+  </si>
+  <si>
+    <t>0:0.01, 30:0.001</t>
+  </si>
+  <si>
+    <t>18-05-16_10-46</t>
+  </si>
+  <si>
+    <t>0:0.01,</t>
+  </si>
+  <si>
+    <t>18-05-16_21-29</t>
+  </si>
+  <si>
+    <t>18-05-16_21-41</t>
+  </si>
+  <si>
+    <t>18-05-17_10-20</t>
+  </si>
+  <si>
+    <t>18-05-17_10-27</t>
+  </si>
+  <si>
+    <t>0:0.001, 150:0.0001</t>
+  </si>
+  <si>
     <t>6-kitchenapp</t>
   </si>
   <si>
@@ -508,9 +538,6 @@
   </si>
   <si>
     <t>18-04-23_20-52_app3</t>
-  </si>
-  <si>
-    <t>0:0.01,</t>
   </si>
   <si>
     <t>18-04-24_10-55_app3</t>
@@ -563,7 +590,7 @@
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -584,11 +611,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -684,7 +706,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -765,10 +787,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V80"/>
+  <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H75" activeCellId="0" sqref="H75"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="49:50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1986,7 +2008,7 @@
       <c r="I32" s="0" t="n">
         <v>-91</v>
       </c>
-      <c r="J32" s="0" t="n">
+      <c r="J32" s="2" t="n">
         <v>0.23</v>
       </c>
       <c r="K32" s="0" t="n">
@@ -2816,7 +2838,7 @@
         <v>105</v>
       </c>
       <c r="N49" s="0" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="O49" s="1"/>
       <c r="P49" s="0" t="n">
@@ -2841,1172 +2863,1237 @@
         <v>150</v>
       </c>
     </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>6.68</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>1.028</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>6.68</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="M50" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="N50" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="P50" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q50" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="R50" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="S50" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="T50" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="U50" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="V50" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="W50" s="0" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M51" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N51" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="P51" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q51" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R51" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="S51" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="T51" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="U51" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="V51" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="n">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>0.0001</v>
+        <v>0.01</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>305</v>
+        <v>10.77</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>488</v>
+        <v>0</v>
       </c>
       <c r="G52" s="0" t="n">
-        <v>444</v>
+        <v>2.02</v>
       </c>
       <c r="H52" s="0" t="n">
-        <v>1.29</v>
+        <v>1.04</v>
       </c>
       <c r="I52" s="0" t="n">
-        <v>305</v>
+        <v>10.77</v>
       </c>
       <c r="J52" s="0" t="n">
-        <v>443</v>
+        <v>1.9</v>
       </c>
       <c r="K52" s="0" t="n">
-        <v>1.29</v>
+        <v>1.02</v>
       </c>
       <c r="M52" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="N52" s="0" t="s">
-        <v>23</v>
+        <v>110</v>
+      </c>
+      <c r="P52" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q52" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R52" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="S52" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="T52" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="U52" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="V52" s="0" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="n">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="C53" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>-67.91</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>22.49</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>-67.91</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M53" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="N53" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="D53" s="0" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="E53" s="0" t="n">
-        <v>-17</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <v>2.64</v>
-      </c>
-      <c r="G53" s="0" t="n">
-        <v>3.61</v>
-      </c>
-      <c r="H53" s="0" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="I53" s="0" t="n">
-        <v>-17</v>
-      </c>
-      <c r="J53" s="0" t="n">
-        <v>2.91</v>
-      </c>
-      <c r="K53" s="0" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="M53" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="N53" s="0" t="s">
-        <v>23</v>
+      <c r="P53" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q53" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R53" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="S53" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="T53" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="U53" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="V53" s="0" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="n">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="C54" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>-72</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>-72</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M54" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="N54" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="D54" s="0" t="n">
-        <v>1E-005</v>
-      </c>
-      <c r="E54" s="0" t="n">
-        <v>4.39</v>
-      </c>
-      <c r="F54" s="0" t="n">
-        <v>0.149</v>
-      </c>
-      <c r="G54" s="0" t="n">
-        <v>2.94</v>
-      </c>
-      <c r="H54" s="0" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="I54" s="0" t="n">
-        <v>4.39</v>
-      </c>
-      <c r="J54" s="0" t="n">
-        <v>2.87</v>
-      </c>
-      <c r="K54" s="0" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="M54" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="N54" s="0" t="s">
-        <v>29</v>
+      <c r="P54" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q54" s="0" t="n">
+        <v>100</v>
       </c>
       <c r="R54" s="0" t="n">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="S54" s="0" t="n">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="T54" s="0" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="U54" s="0" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="V54" s="0" t="n">
-        <v>40</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>-18</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>1.026</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>-18</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="M55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="N55" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="P55" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q55" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R55" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="S55" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="T55" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="U55" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="V55" s="0" t="n">
         <v>150</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D55" s="0" t="n">
-        <v>1E-005</v>
-      </c>
-      <c r="E55" s="0" t="n">
-        <v>-155</v>
-      </c>
-      <c r="F55" s="0" t="n">
-        <v>4.37</v>
-      </c>
-      <c r="G55" s="0" t="n">
-        <v>2.72</v>
-      </c>
-      <c r="H55" s="0" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="I55" s="0" t="n">
-        <v>-171</v>
-      </c>
-      <c r="J55" s="0" t="n">
-        <v>2.12</v>
-      </c>
-      <c r="K55" s="0" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="M55" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="N55" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P55" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q55" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="R55" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="S55" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="T55" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="U55" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="V55" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>1E-005</v>
-      </c>
-      <c r="E56" s="0" t="n">
-        <v>-133</v>
-      </c>
-      <c r="F56" s="0" t="n">
-        <v>7.32</v>
-      </c>
-      <c r="G56" s="0" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="H56" s="0" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="I56" s="0" t="n">
-        <v>-133</v>
-      </c>
-      <c r="J56" s="0" t="n">
-        <v>2.21</v>
-      </c>
-      <c r="K56" s="0" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="M56" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="N56" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="P56" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q56" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="R56" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="S56" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="T56" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="U56" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="V56" s="0" t="n">
-        <v>40</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="n">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>1E-005</v>
+        <v>0.0001</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>-109</v>
+        <v>305</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>1.99</v>
+        <v>488</v>
       </c>
       <c r="G57" s="0" t="n">
-        <v>3.9</v>
+        <v>444</v>
       </c>
       <c r="H57" s="0" t="n">
-        <v>0.79</v>
+        <v>1.29</v>
       </c>
       <c r="I57" s="0" t="n">
-        <v>-109</v>
+        <v>305</v>
       </c>
       <c r="J57" s="0" t="n">
-        <v>2.86</v>
+        <v>443</v>
       </c>
       <c r="K57" s="0" t="n">
-        <v>0.72</v>
+        <v>1.29</v>
       </c>
       <c r="M57" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="N57" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="O57" s="1"/>
-      <c r="P57" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q57" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="R57" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="S57" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="T57" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="U57" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="V57" s="0" t="n">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="n">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>0.0001</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>-77</v>
+        <v>-17</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>1.17</v>
+        <v>2.64</v>
       </c>
       <c r="G58" s="0" t="n">
-        <v>3.3</v>
+        <v>3.61</v>
       </c>
       <c r="H58" s="0" t="n">
-        <v>1.08</v>
+        <v>0.82</v>
       </c>
       <c r="I58" s="0" t="n">
-        <v>-77</v>
+        <v>-17</v>
       </c>
       <c r="J58" s="0" t="n">
-        <v>2.01</v>
+        <v>2.91</v>
       </c>
       <c r="K58" s="0" t="n">
-        <v>0.56</v>
+        <v>0.79</v>
       </c>
       <c r="M58" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="N58" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="O58" s="1"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="n">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>1E-005</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>0.57</v>
+        <v>4.39</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>1.2</v>
+        <v>0.149</v>
       </c>
       <c r="G59" s="0" t="n">
-        <v>2.62</v>
+        <v>2.94</v>
       </c>
       <c r="H59" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I59" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="J59" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="K59" s="0" t="s">
-        <v>74</v>
+        <v>0.66</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <v>4.39</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <v>0.66</v>
       </c>
       <c r="M59" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="N59" s="0" t="s">
-        <v>118</v>
+        <v>29</v>
+      </c>
+      <c r="R59" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S59" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="T59" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U59" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="V59" s="0" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="n">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>1E-005</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>-135</v>
+        <v>-155</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>4.49</v>
+        <v>4.37</v>
       </c>
       <c r="G60" s="0" t="n">
         <v>2.72</v>
       </c>
       <c r="H60" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="J60" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="K60" s="0" t="s">
-        <v>74</v>
+        <v>0.55</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>-171</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>0.49</v>
       </c>
       <c r="M60" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N60" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="O60" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="P60" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q60" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="R60" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S60" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="T60" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U60" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="V60" s="0" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="n">
         <v>200</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="E61" s="2" t="n">
-        <v>-165</v>
+      <c r="E61" s="0" t="n">
+        <v>-133</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>1.51</v>
+        <v>7.32</v>
       </c>
       <c r="G61" s="0" t="n">
-        <v>2.85</v>
+        <v>3.27</v>
       </c>
       <c r="H61" s="0" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="J61" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="K61" s="0" t="s">
-        <v>74</v>
+        <v>0.72</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>-133</v>
+      </c>
+      <c r="J61" s="0" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <v>0.49</v>
       </c>
       <c r="M61" s="0" t="s">
         <v>121</v>
       </c>
       <c r="N61" s="0" t="s">
-        <v>29</v>
+        <v>122</v>
+      </c>
+      <c r="P61" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="R61" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="T61" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U61" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="V61" s="0" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>0.01</v>
+        <v>1E-005</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>31.8</v>
+        <v>-109</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>0</v>
+        <v>1.99</v>
       </c>
       <c r="G62" s="0" t="n">
-        <v>0.83</v>
+        <v>3.9</v>
       </c>
       <c r="H62" s="0" t="n">
-        <v>0.36</v>
+        <v>0.79</v>
       </c>
       <c r="I62" s="0" t="n">
-        <v>-112</v>
+        <v>-109</v>
       </c>
       <c r="J62" s="0" t="n">
-        <v>0.82</v>
+        <v>2.86</v>
       </c>
       <c r="K62" s="0" t="n">
-        <v>0.24</v>
+        <v>0.72</v>
       </c>
       <c r="M62" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N62" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O62" s="1"/>
+      <c r="P62" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q62" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="R62" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S62" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="T62" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U62" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="V62" s="0" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>0.01</v>
+        <v>0.0001</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>-130.83</v>
+        <v>-77</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="G63" s="2" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="H63" s="2" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="I63" s="2" t="n">
-        <v>-181</v>
+        <v>1.17</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>-77</v>
       </c>
       <c r="J63" s="0" t="n">
-        <v>0.43</v>
+        <v>2.01</v>
       </c>
       <c r="K63" s="0" t="n">
-        <v>0.17</v>
+        <v>0.56</v>
       </c>
       <c r="M63" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N63" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="P63" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="Q63" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="R63" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="S63" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="T63" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="O63" s="1"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="M64" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="N64" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="U63" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="V63" s="0" t="n">
-        <v>150</v>
-      </c>
+      <c r="C65" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>-135</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <v>2.72</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="M65" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="N65" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="O65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="n">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="E66" s="0" t="n">
-        <v>-37</v>
+        <v>1E-005</v>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>-165</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>1.32</v>
+        <v>1.51</v>
       </c>
       <c r="G66" s="0" t="n">
-        <v>0.98</v>
+        <v>2.85</v>
       </c>
       <c r="H66" s="0" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="I66" s="0" t="n">
-        <v>-46</v>
-      </c>
-      <c r="J66" s="0" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="K66" s="0" t="n">
-        <v>0.42</v>
+        <v>0.66</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="M66" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="N66" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="P66" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q66" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="R66" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="S66" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="T66" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="U66" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="V66" s="0" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>0.01</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>66</v>
+        <v>31.8</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>2E-005</v>
+        <v>0</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>0.237</v>
+        <v>0.83</v>
       </c>
       <c r="H67" s="0" t="n">
-        <v>0.237</v>
+        <v>0.36</v>
       </c>
       <c r="I67" s="0" t="n">
-        <v>-89</v>
+        <v>-112</v>
       </c>
       <c r="J67" s="0" t="n">
-        <v>0.237</v>
+        <v>0.82</v>
       </c>
       <c r="K67" s="0" t="n">
-        <v>0.161</v>
+        <v>0.24</v>
       </c>
       <c r="M67" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N67" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="O67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>-130.83</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G68" s="2" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H68" s="2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="I68" s="2" t="n">
+        <v>-181</v>
+      </c>
+      <c r="J68" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="K68" s="0" t="n">
+        <v>0.17</v>
+      </c>
       <c r="M68" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="N68" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="D70" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="P68" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q68" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="R68" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="S68" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="T68" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="U68" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="V68" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="E70" s="0" t="n">
-        <v>-19</v>
-      </c>
-      <c r="F70" s="0" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="G70" s="0" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="H70" s="0" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="I70" s="0" t="n">
-        <v>-60</v>
-      </c>
-      <c r="J70" s="0" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="K70" s="0" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="M70" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="N70" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q70" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="R70" s="0" t="n">
+      <c r="E71" s="0" t="n">
+        <v>-37</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>-46</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="K71" s="0" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M71" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="N71" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="P71" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q71" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="S70" s="0" t="n">
+      <c r="R71" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="S71" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="T71" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="T70" s="0" t="n">
+      <c r="U71" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="U70" s="0" t="n">
+      <c r="V71" s="0" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>1E-005</v>
+        <v>0.01</v>
       </c>
       <c r="E72" s="0" t="n">
-        <v>156</v>
+        <v>66</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>0.07</v>
+        <v>2E-005</v>
       </c>
       <c r="G72" s="0" t="n">
-        <v>2.5</v>
+        <v>0.237</v>
       </c>
       <c r="H72" s="0" t="n">
-        <v>0.96</v>
+        <v>0.237</v>
       </c>
       <c r="I72" s="0" t="n">
-        <v>156</v>
+        <v>-89</v>
       </c>
       <c r="J72" s="0" t="n">
-        <v>2.5</v>
+        <v>0.237</v>
       </c>
       <c r="K72" s="0" t="n">
-        <v>0.96</v>
+        <v>0.161</v>
       </c>
       <c r="M72" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="N72" s="0" t="s">
-        <v>29</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="O72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D73" s="0" t="n">
-        <v>1E-005</v>
-      </c>
-      <c r="E73" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="G73" s="0" t="n">
-        <v>2.87</v>
-      </c>
-      <c r="H73" s="0" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="I73" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="J73" s="0" t="n">
-        <v>2.67</v>
-      </c>
-      <c r="K73" s="0" t="n">
-        <v>0.84</v>
-      </c>
       <c r="M73" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N73" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D74" s="0" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="E74" s="0" t="n">
-        <v>-93</v>
-      </c>
-      <c r="F74" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G74" s="0" t="n">
-        <v>2.31</v>
-      </c>
-      <c r="H74" s="0" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I74" s="0" t="n">
-        <v>-93</v>
-      </c>
-      <c r="J74" s="0" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="K74" s="0" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="M74" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="N74" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="n">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>0.0001</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>-128</v>
+        <v>-19</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>1.37</v>
+        <v>0.25</v>
       </c>
       <c r="G75" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H75" s="2" t="n">
-        <v>0.37</v>
+        <v>1.04</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <v>0.43</v>
       </c>
       <c r="I75" s="0" t="n">
-        <v>-235</v>
+        <v>-60</v>
       </c>
       <c r="J75" s="0" t="n">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="K75" s="0" t="n">
-        <v>0.37</v>
+        <v>0.4</v>
       </c>
       <c r="M75" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="N75" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="P75" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="Q75" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="R75" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="Q75" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="R75" s="0" t="n">
-        <v>150</v>
-      </c>
       <c r="S75" s="0" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="T75" s="0" t="n">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="U75" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="V75" s="0" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D76" s="0" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="E76" s="2" t="n">
-        <v>-169</v>
-      </c>
-      <c r="F76" s="0" t="n">
-        <v>2.06</v>
-      </c>
-      <c r="G76" s="0" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="H76" s="0" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I76" s="0" t="n">
-        <v>-262</v>
-      </c>
-      <c r="J76" s="0" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="K76" s="0" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="M76" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="N76" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="P76" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q76" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="R76" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="S76" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="T76" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="U76" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="V76" s="0" t="n">
-        <v>150</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>0.0001</v>
+        <v>1E-005</v>
       </c>
       <c r="E77" s="0" t="n">
-        <v>-77</v>
+        <v>156</v>
       </c>
       <c r="F77" s="0" t="n">
-        <v>1.69</v>
+        <v>0.07</v>
       </c>
       <c r="G77" s="0" t="n">
-        <v>0.82</v>
+        <v>2.5</v>
       </c>
       <c r="H77" s="0" t="n">
-        <v>0.38</v>
+        <v>0.96</v>
       </c>
       <c r="I77" s="0" t="n">
-        <v>-255</v>
+        <v>156</v>
       </c>
       <c r="J77" s="0" t="n">
-        <v>0.82</v>
+        <v>2.5</v>
       </c>
       <c r="K77" s="0" t="n">
-        <v>0.36</v>
+        <v>0.96</v>
       </c>
       <c r="M77" s="0" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="N77" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="P77" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="Q77" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="R77" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="S77" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="T77" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="U77" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="V77" s="0" t="n">
-        <v>250</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>0.0001</v>
+        <v>1E-005</v>
       </c>
       <c r="E78" s="0" t="n">
-        <v>245</v>
+        <v>11</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>2.56</v>
+        <v>0.16</v>
       </c>
       <c r="G78" s="0" t="n">
-        <v>0.89</v>
+        <v>2.87</v>
       </c>
       <c r="H78" s="0" t="n">
-        <v>0.44</v>
+        <v>0.84</v>
       </c>
       <c r="I78" s="0" t="n">
-        <v>-198</v>
+        <v>11</v>
       </c>
       <c r="J78" s="0" t="n">
-        <v>0.79</v>
+        <v>2.67</v>
       </c>
       <c r="K78" s="0" t="n">
-        <v>0.34</v>
+        <v>0.84</v>
       </c>
       <c r="M78" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="N78" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="P78" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="Q78" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="R78" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="S78" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="T78" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="U78" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="V78" s="0" t="n">
-        <v>250</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>0.01</v>
+        <v>0.0001</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>32.534</v>
+        <v>-93</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="G79" s="2" t="n">
-        <v>0.7</v>
+        <v>0.1</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>2.31</v>
       </c>
       <c r="H79" s="0" t="n">
-        <v>0.48</v>
+        <v>0.75</v>
       </c>
       <c r="I79" s="0" t="n">
-        <v>-9.41</v>
+        <v>-93</v>
       </c>
       <c r="J79" s="0" t="n">
-        <v>0.51</v>
+        <v>2.3</v>
       </c>
       <c r="K79" s="0" t="n">
-        <v>0.39</v>
+        <v>0.75</v>
       </c>
       <c r="M79" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="N79" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="P79" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="Q79" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="R79" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="S79" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="T79" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="U79" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="V79" s="0" t="n">
-        <v>150</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>0.01</v>
+        <v>0.0001</v>
       </c>
       <c r="E80" s="0" t="n">
-        <v>13.6142</v>
+        <v>-128</v>
       </c>
       <c r="F80" s="0" t="n">
-        <v>0.0002</v>
+        <v>1.37</v>
       </c>
       <c r="G80" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="H80" s="0" t="n">
-        <v>0.52</v>
+        <v>0.9</v>
+      </c>
+      <c r="H80" s="2" t="n">
+        <v>0.37</v>
       </c>
       <c r="I80" s="0" t="n">
-        <v>-33</v>
+        <v>-235</v>
       </c>
       <c r="J80" s="0" t="n">
-        <v>0.56</v>
+        <v>0.9</v>
       </c>
       <c r="K80" s="0" t="n">
-        <v>0.4</v>
+        <v>0.37</v>
       </c>
       <c r="M80" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="N80" s="0" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="P80" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="Q80" s="0" t="n">
         <v>80</v>
@@ -4024,6 +4111,301 @@
         <v>250</v>
       </c>
       <c r="V80" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>-169</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <v>-262</v>
+      </c>
+      <c r="J81" s="0" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="K81" s="0" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M81" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="N81" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P81" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q81" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="R81" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="S81" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="T81" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="U81" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="V81" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>-77</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <v>-255</v>
+      </c>
+      <c r="J82" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="K82" s="0" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M82" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="N82" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P82" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q82" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="R82" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="S82" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="T82" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="U82" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="V82" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>-198</v>
+      </c>
+      <c r="J83" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="K83" s="0" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M83" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="N83" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="P83" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q83" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="R83" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="S83" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="T83" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="U83" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="V83" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>32.534</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G84" s="2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>-9.41</v>
+      </c>
+      <c r="J84" s="0" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="K84" s="0" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M84" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="N84" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="P84" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q84" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="R84" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="S84" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="T84" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="U84" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="V84" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>13.6142</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="G85" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <v>-33</v>
+      </c>
+      <c r="J85" s="0" t="n">
+        <v>0.56</v>
+      </c>
+      <c r="K85" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="M85" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="N85" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="P85" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q85" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="R85" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="S85" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="T85" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="U85" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="V85" s="0" t="n">
         <v>150</v>
       </c>
     </row>
@@ -4045,8 +4427,8 @@
   </sheetPr>
   <dimension ref="A1:U65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q8" activeCellId="0" sqref="Q8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q8" activeCellId="1" sqref="49:50 Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
@@ -4060,7 +4442,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>0</v>
@@ -4128,7 +4510,7 @@
         <v>2859</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>100</v>
@@ -4158,10 +4540,10 @@
         <v>0.25</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>80</v>
@@ -4190,7 +4572,7 @@
         <v>2859</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>100</v>
@@ -4220,10 +4602,10 @@
         <v>0.25</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="Q3" s="0" t="n">
         <v>150</v>
@@ -4246,7 +4628,7 @@
         <v>2859</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>100</v>
@@ -4276,10 +4658,10 @@
         <v>0.19</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="O4" s="0" t="n">
         <v>60</v>
@@ -4308,7 +4690,7 @@
         <v>2859</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>200</v>
@@ -4338,10 +4720,10 @@
         <v>0.27</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="Q5" s="0" t="n">
         <v>150</v>
@@ -4364,7 +4746,7 @@
         <v>2859</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>200</v>
@@ -4394,10 +4776,10 @@
         <v>0.23</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4405,7 +4787,7 @@
         <v>2859</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>300</v>
@@ -4435,10 +4817,10 @@
         <v>0.31</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="Q7" s="0" t="n">
         <v>150</v>
@@ -4461,7 +4843,7 @@
         <v>2859</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>300</v>
@@ -4491,10 +4873,10 @@
         <v>0.23</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="O8" s="0" t="n">
         <v>150</v>
@@ -4527,7 +4909,7 @@
         <v>6990</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>100</v>
@@ -4557,10 +4939,10 @@
         <v>0.3</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4568,7 +4950,7 @@
         <v>6990</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>120</v>
@@ -4612,10 +4994,10 @@
         <v>0.14</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4653,10 +5035,10 @@
         <v>0.21</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4694,10 +5076,10 @@
         <v>0.13</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="O19" s="0" t="n">
         <v>80</v>
@@ -4756,10 +5138,10 @@
         <v>0.08</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,10 +5179,10 @@
         <v>0.22</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="Q21" s="0" t="n">
         <v>100</v>
@@ -4853,10 +5235,10 @@
         <v>0.09</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="O22" s="0" t="n">
         <v>80</v>
@@ -4915,10 +5297,10 @@
         <v>0.11</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="O23" s="0" t="n">
         <v>80</v>
@@ -4962,10 +5344,10 @@
         <v>0.14</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5003,10 +5385,10 @@
         <v>0.19</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5044,10 +5426,10 @@
         <v>0.31</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5085,10 +5467,10 @@
         <v>0.34</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="Q30" s="0" t="n">
         <v>100</v>

</xml_diff>